<commit_message>
Ensure latest local changes are captured before moving to github.
</commit_message>
<xml_diff>
--- a/docs/Parts List.xlsx
+++ b/docs/Parts List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EasiBuild Mk 2" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="621">
   <si>
     <t>EasiBuild Mark 2 Parts</t>
   </si>
@@ -1892,6 +1892,12 @@
   </si>
   <si>
     <t>orig 1000</t>
+  </si>
+  <si>
+    <t>0.01 is a 103</t>
+  </si>
+  <si>
+    <t>0.1 is a 104 which I used.</t>
   </si>
 </sst>
 </file>
@@ -4766,7 +4772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I255"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -13477,10 +13483,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13488,12 +13494,12 @@
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1500</v>
       </c>
@@ -13501,17 +13507,17 @@
         <v>618</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>433</v>
       </c>
@@ -13519,7 +13525,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>0.01</v>
       </c>
@@ -13527,30 +13533,38 @@
         <f>A8*(10^-6)</f>
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D8" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11" s="29">
         <f>1 / (2 * PI() * A2)</f>
         <v>1.061032953945969E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" s="31">
         <f>A11/B8</f>
         <v>10610.32953945969</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>437</v>
       </c>

</xml_diff>